<commit_message>
add autoreport info table write to excel
</commit_message>
<xml_diff>
--- a/I2C_Template_20230414.xlsx
+++ b/I2C_Template_20230414.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9984B47E-05B8-404C-B375-9FB3D1FE72B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB23319F-82B6-46E3-96D5-E22C36C7270E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="65085" yWindow="1710" windowWidth="19500" windowHeight="11400" tabRatio="687" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="59490" yWindow="2685" windowWidth="25200" windowHeight="10605" tabRatio="687" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master-Chip_100kHz" sheetId="11" r:id="rId1"/>
     <sheet name="Master-Chip_400kHz" sheetId="10" r:id="rId2"/>
     <sheet name="Master-Chip_1000kHz" sheetId="12" r:id="rId3"/>
     <sheet name="Basic" sheetId="13" r:id="rId4"/>
+    <sheet name="Testing" sheetId="14" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="192">
   <si>
     <t>Parameter</t>
     <phoneticPr fontId="7" type="noConversion"/>
@@ -176,24 +177,6 @@
   </si>
   <si>
     <t>Jaws</t>
-  </si>
-  <si>
-    <t>Parameter</t>
-  </si>
-  <si>
-    <t>Net Name</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>0</t>
   </si>
   <si>
     <t>Project Name</t>
@@ -868,7 +851,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -953,6 +936,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1256,7 +1245,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1292,7 +1281,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1346,6 +1334,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="115">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1742,18 +1739,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14D51BD-4D05-44CA-9BB1-ED1C5AFF2395}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.7"/>
   <cols>
-    <col min="1" max="1" width="22.4375" style="26" customWidth="1"/>
-    <col min="2" max="2" width="19.75" style="26" customWidth="1"/>
-    <col min="3" max="3" width="15" style="26" customWidth="1"/>
-    <col min="4" max="6" width="9" style="26"/>
-    <col min="7" max="7" width="14.125" style="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="26"/>
+    <col min="1" max="1" width="22.4375" style="25" customWidth="1"/>
+    <col min="2" max="2" width="19.75" style="25" customWidth="1"/>
+    <col min="3" max="3" width="15" style="25" customWidth="1"/>
+    <col min="4" max="6" width="9" style="25"/>
+    <col min="7" max="7" width="14.125" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1780,333 +1777,333 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="28">
+      <c r="D2" s="27">
         <v>1.26</v>
       </c>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28" t="s">
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="27">
         <v>-0.5</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28">
+      <c r="E3" s="27"/>
+      <c r="F3" s="27">
         <v>0.54</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="27" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="27">
         <v>1.26</v>
       </c>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28" t="s">
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="27">
         <v>-0.5</v>
       </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28">
+      <c r="E5" s="27"/>
+      <c r="F5" s="27">
         <v>0.54</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="27" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="27">
         <v>4.7</v>
       </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28" t="s">
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="27">
         <v>4</v>
       </c>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28" t="s">
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="27">
         <v>0</v>
       </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28">
+      <c r="E8" s="27"/>
+      <c r="F8" s="27">
         <v>200</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="27" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="B9" s="27" t="s">
+      <c r="A9" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="B9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28">
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27">
         <v>1000</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="27" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="27" t="s">
-        <v>195</v>
-      </c>
-      <c r="B10" s="27" t="s">
+      <c r="A10" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="B10" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28">
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27">
         <v>300</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="27" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="B11" s="27" t="s">
+      <c r="A11" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28">
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27">
         <v>1000</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="27" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="27" t="s">
-        <v>195</v>
-      </c>
-      <c r="B12" s="27" t="s">
+      <c r="A12" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="B12" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="27">
         <v>20</v>
       </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28">
+      <c r="E12" s="27"/>
+      <c r="F12" s="27">
         <v>300</v>
       </c>
-      <c r="G12" s="28" t="s">
+      <c r="G12" s="27" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D13" s="27">
         <v>250</v>
       </c>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28" t="s">
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="28">
+      <c r="D14" s="27">
         <v>0</v>
       </c>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28" t="s">
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="32" customFormat="1">
-      <c r="A15" s="29" t="s">
+    <row r="15" spans="1:7" s="31" customFormat="1">
+      <c r="A15" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="31">
+      <c r="D15" s="30">
         <v>4.7</v>
       </c>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31" t="s">
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="32" customFormat="1">
-      <c r="A16" s="27" t="s">
+    <row r="16" spans="1:7" s="31" customFormat="1">
+      <c r="A16" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="31">
+      <c r="D16" s="30">
         <v>4</v>
       </c>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31" t="s">
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="27" t="s">
-        <v>196</v>
-      </c>
-      <c r="D17" s="31">
+      <c r="C17" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="D17" s="30">
         <v>4</v>
       </c>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31" t="s">
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="30" t="s">
-        <v>175</v>
-      </c>
-      <c r="B18" s="30" t="s">
+      <c r="A18" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="B18" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="27" t="s">
-        <v>197</v>
-      </c>
-      <c r="D18" s="31">
+      <c r="C18" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="D18" s="30">
         <v>4.7</v>
       </c>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31" t="s">
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2463,8 +2460,8 @@
       <c r="B17" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="27" t="s">
-        <v>196</v>
+      <c r="C17" s="26" t="s">
+        <v>190</v>
       </c>
       <c r="D17" s="10">
         <v>0.6</v>
@@ -2477,13 +2474,13 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="8" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="27" t="s">
-        <v>197</v>
+      <c r="C18" s="26" t="s">
+        <v>191</v>
       </c>
       <c r="D18" s="10">
         <v>1.3</v>
@@ -2542,7 +2539,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
@@ -2561,7 +2558,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -2582,7 +2579,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>10</v>
@@ -2601,7 +2598,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
@@ -2681,7 +2678,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
@@ -2838,8 +2835,8 @@
       <c r="B17" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="27" t="s">
-        <v>196</v>
+      <c r="C17" s="26" t="s">
+        <v>190</v>
       </c>
       <c r="D17" s="10">
         <v>0.26</v>
@@ -2857,8 +2854,8 @@
       <c r="B18" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="27" t="s">
-        <v>197</v>
+      <c r="C18" s="26" t="s">
+        <v>191</v>
       </c>
       <c r="D18" s="10">
         <v>0.5</v>
@@ -2878,878 +2875,1414 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3000E240-3F1F-4EAA-8673-94E43FB6958A}">
-  <dimension ref="A1:K134"/>
+  <dimension ref="A1:B134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.7"/>
   <cols>
-    <col min="1" max="1" width="32.625" style="25" customWidth="1"/>
-    <col min="2" max="2" width="49" style="24" customWidth="1"/>
-    <col min="3" max="3" width="2.375" customWidth="1"/>
-    <col min="4" max="4" width="2.75" customWidth="1"/>
-    <col min="5" max="5" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.25" customWidth="1"/>
+    <col min="1" max="1" width="32.625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="49" style="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="31.35">
+      <c r="A5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="62.7">
+      <c r="A9" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="12"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="12"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="12"/>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="12"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="12"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="12"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="12"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="12"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="12"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="19"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="19"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="19"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="19"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="19"/>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="19"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" s="19"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" s="19"/>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="19"/>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" s="19"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" s="12"/>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" s="12"/>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="12"/>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" s="12"/>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" s="12"/>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="12"/>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" s="12"/>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" s="12"/>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" s="12"/>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B45" s="12"/>
+    </row>
+    <row r="46" spans="1:2" ht="94">
+      <c r="A46" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="31.35">
+      <c r="A47" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="203.7">
+      <c r="A48" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="31.35">
+      <c r="A49" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="203.7">
+      <c r="A50" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="31.35">
+      <c r="A51" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="203.7">
+      <c r="A52" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="31.35">
+      <c r="A53" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="203.7">
+      <c r="A54" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="31.35">
+      <c r="A55" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="203.7">
+      <c r="A56" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="31.35">
+      <c r="A57" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="203.7">
+      <c r="A58" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="31.35">
+      <c r="A59" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="94">
+      <c r="A60" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="31.35">
+      <c r="A61" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="94">
+      <c r="A62" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="31.35">
+      <c r="A63" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="B63" s="13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="94">
+      <c r="A64" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="31.35">
+      <c r="A65" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="94">
+      <c r="A66" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="B66" s="13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="31.35">
+      <c r="A67" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="B67" s="13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="94">
+      <c r="A68" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B68" s="13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="31.35">
+      <c r="A69" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="B69" s="13" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="94">
+      <c r="A70" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="B70" s="13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="31.35">
+      <c r="A71" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="B71" s="13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="B72" s="13"/>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="B73" s="13"/>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B74" s="13"/>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="B75" s="13"/>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="B76" s="13"/>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="B77" s="13"/>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="B78" s="13"/>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="B79" s="13"/>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="B80" s="13"/>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="B81" s="13"/>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="B82" s="13"/>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="B83" s="13"/>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B84" s="13"/>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="B85" s="13"/>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B86" s="12"/>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B87" s="12"/>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B88" s="12"/>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B89" s="12"/>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B90" s="12"/>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B91" s="12"/>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B92" s="12"/>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B93" s="12"/>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B94" s="12"/>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B95" s="12"/>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B96" s="12"/>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B97" s="12"/>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B98" s="12"/>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B99" s="12"/>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B100" s="12"/>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B101" s="12"/>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B102" s="12"/>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="B103" s="12"/>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="B104" s="12"/>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B105" s="12"/>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B106" s="12"/>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B107" s="12"/>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B108" s="12"/>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B109" s="12"/>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="B110" s="12"/>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B111" s="12"/>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B112" s="12"/>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B113" s="12"/>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B114" s="12"/>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="B115" s="12"/>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="22"/>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="22"/>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="22"/>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="22"/>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="22"/>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="22"/>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="22"/>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="22"/>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="22"/>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="22"/>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="22"/>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="22"/>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="22"/>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" s="22"/>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" s="22"/>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="22"/>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" s="22"/>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" s="22"/>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="22"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF5FF9B1-5F08-424A-A901-D19774BA9A4A}">
+  <dimension ref="A1:K134"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.7"/>
+  <cols>
+    <col min="1" max="1" width="32.625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="49" style="34" customWidth="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
+    <col min="6" max="6" width="14.75" customWidth="1"/>
+    <col min="7" max="7" width="13.375" customWidth="1"/>
+    <col min="8" max="8" width="12.6875" customWidth="1"/>
+    <col min="9" max="9" width="12.25" customWidth="1"/>
+    <col min="10" max="10" width="10.5625" customWidth="1"/>
+    <col min="11" max="11" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" s="13" t="s">
+      <c r="A1" s="11"/>
+      <c r="B1" s="32"/>
+      <c r="E1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>49</v>
-      </c>
+      <c r="A2" s="11"/>
+      <c r="B2" s="32"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>51</v>
-      </c>
+      <c r="A3" s="11"/>
+      <c r="B3" s="32"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="31.35">
-      <c r="A5" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>55</v>
-      </c>
+      <c r="A4" s="11"/>
+      <c r="B4" s="32"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="11"/>
+      <c r="B5" s="32"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>57</v>
-      </c>
+      <c r="A6" s="11"/>
+      <c r="B6" s="32"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>59</v>
-      </c>
+      <c r="A7" s="14"/>
+      <c r="B7" s="32"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="62.7">
-      <c r="A9" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>63</v>
-      </c>
+      <c r="A8" s="14"/>
+      <c r="B8" s="32"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="14"/>
+      <c r="B9" s="32"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>65</v>
-      </c>
+      <c r="A10" s="14"/>
+      <c r="B10" s="32"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>67</v>
-      </c>
+      <c r="A11" s="14"/>
+      <c r="B11" s="32"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>69</v>
-      </c>
+      <c r="A12" s="14"/>
+      <c r="B12" s="32"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="12"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="32"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" s="12"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="32"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="B15" s="12"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="32"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="B16" s="12"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="32"/>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="12"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="32"/>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="12"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="32"/>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" s="12"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="32"/>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="B20" s="12"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="32"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" s="12"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="32"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>80</v>
-      </c>
+      <c r="A22" s="15"/>
+      <c r="B22" s="32"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>51</v>
-      </c>
+      <c r="A23" s="16"/>
+      <c r="B23" s="32"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>80</v>
-      </c>
+      <c r="A24" s="16"/>
+      <c r="B24" s="33"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>84</v>
-      </c>
+      <c r="A25" s="16"/>
+      <c r="B25" s="33"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="B26" s="20"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="33"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="B27" s="20"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="33"/>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="B28" s="20"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="33"/>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="B29" s="20"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="33"/>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="B30" s="20"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="33"/>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B31" s="20"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="33"/>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="B32" s="20"/>
+      <c r="A32" s="18"/>
+      <c r="B32" s="33"/>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="B33" s="20"/>
+      <c r="A33" s="18"/>
+      <c r="B33" s="33"/>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="B34" s="20"/>
+      <c r="A34" s="18"/>
+      <c r="B34" s="33"/>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="B35" s="20"/>
+      <c r="A35" s="18"/>
+      <c r="B35" s="33"/>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="B36" s="12"/>
+      <c r="A36" s="20"/>
+      <c r="B36" s="32"/>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="B37" s="12"/>
+      <c r="A37" s="20"/>
+      <c r="B37" s="32"/>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="B38" s="12"/>
+      <c r="A38" s="20"/>
+      <c r="B38" s="32"/>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="B39" s="12"/>
+      <c r="A39" s="20"/>
+      <c r="B39" s="32"/>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="B40" s="12"/>
+      <c r="A40" s="20"/>
+      <c r="B40" s="32"/>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="B41" s="12"/>
+      <c r="A41" s="20"/>
+      <c r="B41" s="32"/>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="B42" s="12"/>
+      <c r="A42" s="20"/>
+      <c r="B42" s="32"/>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="B43" s="12"/>
+      <c r="A43" s="20"/>
+      <c r="B43" s="32"/>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="B44" s="12"/>
+      <c r="A44" s="20"/>
+      <c r="B44" s="32"/>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="B45" s="12"/>
-    </row>
-    <row r="46" spans="1:2" ht="94">
-      <c r="A46" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="31.35">
-      <c r="A47" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="B47" s="14" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="203.7">
-      <c r="A48" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="B48" s="14" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="31.35">
-      <c r="A49" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="203.7">
-      <c r="A50" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="B50" s="14" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="31.35">
-      <c r="A51" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="B51" s="14" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="203.7">
-      <c r="A52" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="B52" s="14" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="31.35">
-      <c r="A53" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="B53" s="14" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="203.7">
-      <c r="A54" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="B54" s="14" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="31.35">
-      <c r="A55" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="B55" s="14" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="203.7">
-      <c r="A56" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="B56" s="14" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="31.35">
-      <c r="A57" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="B57" s="14" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="203.7">
-      <c r="A58" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="B58" s="14" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="31.35">
-      <c r="A59" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="B59" s="14" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="94">
-      <c r="A60" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="B60" s="14" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="31.35">
-      <c r="A61" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="B61" s="14" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="94">
-      <c r="A62" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="B62" s="14" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="31.35">
-      <c r="A63" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="B63" s="14" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="94">
-      <c r="A64" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="B64" s="14" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="31.35">
-      <c r="A65" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="B65" s="14" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="94">
-      <c r="A66" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="B66" s="14" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="31.35">
-      <c r="A67" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="B67" s="14" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="94">
-      <c r="A68" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="B68" s="14" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="31.35">
-      <c r="A69" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="B69" s="14" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="94">
-      <c r="A70" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="B70" s="14" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="31.35">
-      <c r="A71" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="B71" s="14" t="s">
-        <v>191</v>
-      </c>
+      <c r="A45" s="20"/>
+      <c r="B45" s="32"/>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="21"/>
+      <c r="B46" s="32"/>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="21"/>
+      <c r="B47" s="32"/>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="21"/>
+      <c r="B48" s="32"/>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="21"/>
+      <c r="B49" s="32"/>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="21"/>
+      <c r="B50" s="32"/>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="21"/>
+      <c r="B51" s="32"/>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="21"/>
+      <c r="B52" s="32"/>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="21"/>
+      <c r="B53" s="32"/>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="21"/>
+      <c r="B54" s="32"/>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="21"/>
+      <c r="B55" s="32"/>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="21"/>
+      <c r="B56" s="32"/>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="21"/>
+      <c r="B57" s="32"/>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="21"/>
+      <c r="B58" s="32"/>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="21"/>
+      <c r="B59" s="32"/>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="21"/>
+      <c r="B60" s="32"/>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="21"/>
+      <c r="B61" s="32"/>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="21"/>
+      <c r="B62" s="32"/>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="21"/>
+      <c r="B63" s="32"/>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="21"/>
+      <c r="B64" s="32"/>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="21"/>
+      <c r="B65" s="32"/>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="21"/>
+      <c r="B66" s="32"/>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="21"/>
+      <c r="B67" s="32"/>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="21"/>
+      <c r="B68" s="32"/>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="21"/>
+      <c r="B69" s="32"/>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="21"/>
+      <c r="B70" s="32"/>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="21"/>
+      <c r="B71" s="32"/>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="B72" s="14"/>
+      <c r="A72" s="21"/>
+      <c r="B72" s="32"/>
     </row>
     <row r="73" spans="1:2">
-      <c r="A73" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="B73" s="14"/>
+      <c r="A73" s="21"/>
+      <c r="B73" s="32"/>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="B74" s="14"/>
+      <c r="A74" s="21"/>
+      <c r="B74" s="32"/>
     </row>
     <row r="75" spans="1:2">
-      <c r="A75" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="B75" s="14"/>
+      <c r="A75" s="21"/>
+      <c r="B75" s="32"/>
     </row>
     <row r="76" spans="1:2">
-      <c r="A76" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="B76" s="14"/>
+      <c r="A76" s="21"/>
+      <c r="B76" s="32"/>
     </row>
     <row r="77" spans="1:2">
-      <c r="A77" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="B77" s="14"/>
+      <c r="A77" s="21"/>
+      <c r="B77" s="32"/>
     </row>
     <row r="78" spans="1:2">
-      <c r="A78" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="B78" s="14"/>
+      <c r="A78" s="21"/>
+      <c r="B78" s="32"/>
     </row>
     <row r="79" spans="1:2">
-      <c r="A79" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="B79" s="14"/>
+      <c r="A79" s="21"/>
+      <c r="B79" s="32"/>
     </row>
     <row r="80" spans="1:2">
-      <c r="A80" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="B80" s="14"/>
+      <c r="A80" s="21"/>
+      <c r="B80" s="32"/>
     </row>
     <row r="81" spans="1:2">
-      <c r="A81" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="B81" s="14"/>
+      <c r="A81" s="21"/>
+      <c r="B81" s="32"/>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="B82" s="14"/>
+      <c r="A82" s="21"/>
+      <c r="B82" s="32"/>
     </row>
     <row r="83" spans="1:2">
-      <c r="A83" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="B83" s="14"/>
+      <c r="A83" s="21"/>
+      <c r="B83" s="32"/>
     </row>
     <row r="84" spans="1:2">
-      <c r="A84" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="B84" s="14"/>
+      <c r="A84" s="21"/>
+      <c r="B84" s="32"/>
     </row>
     <row r="85" spans="1:2">
-      <c r="A85" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="B85" s="14"/>
+      <c r="A85" s="21"/>
+      <c r="B85" s="32"/>
     </row>
     <row r="86" spans="1:2">
-      <c r="A86" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="B86" s="12"/>
+      <c r="A86" s="11"/>
+      <c r="B86" s="32"/>
     </row>
     <row r="87" spans="1:2">
-      <c r="A87" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="B87" s="12"/>
+      <c r="A87" s="11"/>
+      <c r="B87" s="32"/>
     </row>
     <row r="88" spans="1:2">
-      <c r="A88" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="B88" s="12"/>
+      <c r="A88" s="11"/>
+      <c r="B88" s="32"/>
     </row>
     <row r="89" spans="1:2">
-      <c r="A89" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="B89" s="12"/>
+      <c r="A89" s="11"/>
+      <c r="B89" s="32"/>
     </row>
     <row r="90" spans="1:2">
-      <c r="A90" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="B90" s="12"/>
+      <c r="A90" s="11"/>
+      <c r="B90" s="32"/>
     </row>
     <row r="91" spans="1:2">
-      <c r="A91" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="B91" s="12"/>
+      <c r="A91" s="11"/>
+      <c r="B91" s="32"/>
     </row>
     <row r="92" spans="1:2">
-      <c r="A92" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="B92" s="12"/>
+      <c r="A92" s="11"/>
+      <c r="B92" s="32"/>
     </row>
     <row r="93" spans="1:2">
-      <c r="A93" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="B93" s="12"/>
+      <c r="A93" s="11"/>
+      <c r="B93" s="32"/>
     </row>
     <row r="94" spans="1:2">
-      <c r="A94" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="B94" s="12"/>
+      <c r="A94" s="11"/>
+      <c r="B94" s="32"/>
     </row>
     <row r="95" spans="1:2">
-      <c r="A95" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="B95" s="12"/>
+      <c r="A95" s="11"/>
+      <c r="B95" s="32"/>
     </row>
     <row r="96" spans="1:2">
-      <c r="A96" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="B96" s="12"/>
+      <c r="A96" s="11"/>
+      <c r="B96" s="32"/>
     </row>
     <row r="97" spans="1:2">
-      <c r="A97" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="B97" s="12"/>
+      <c r="A97" s="11"/>
+      <c r="B97" s="32"/>
     </row>
     <row r="98" spans="1:2">
-      <c r="A98" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="B98" s="12"/>
+      <c r="A98" s="11"/>
+      <c r="B98" s="32"/>
     </row>
     <row r="99" spans="1:2">
-      <c r="A99" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="B99" s="12"/>
+      <c r="A99" s="11"/>
+      <c r="B99" s="32"/>
     </row>
     <row r="100" spans="1:2">
-      <c r="A100" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="B100" s="12"/>
+      <c r="A100" s="11"/>
+      <c r="B100" s="32"/>
     </row>
     <row r="101" spans="1:2">
-      <c r="A101" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="B101" s="12"/>
+      <c r="A101" s="11"/>
+      <c r="B101" s="32"/>
     </row>
     <row r="102" spans="1:2">
-      <c r="A102" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="B102" s="12"/>
+      <c r="A102" s="11"/>
+      <c r="B102" s="32"/>
     </row>
     <row r="103" spans="1:2">
-      <c r="A103" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B103" s="12"/>
+      <c r="A103" s="11"/>
+      <c r="B103" s="32"/>
     </row>
     <row r="104" spans="1:2">
-      <c r="A104" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="B104" s="12"/>
+      <c r="A104" s="11"/>
+      <c r="B104" s="32"/>
     </row>
     <row r="105" spans="1:2">
-      <c r="A105" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="B105" s="12"/>
+      <c r="A105" s="11"/>
+      <c r="B105" s="32"/>
     </row>
     <row r="106" spans="1:2">
-      <c r="A106" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="B106" s="12"/>
+      <c r="A106" s="11"/>
+      <c r="B106" s="32"/>
     </row>
     <row r="107" spans="1:2">
-      <c r="A107" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="B107" s="12"/>
+      <c r="A107" s="11"/>
+      <c r="B107" s="32"/>
     </row>
     <row r="108" spans="1:2">
-      <c r="A108" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="B108" s="12"/>
+      <c r="A108" s="11"/>
+      <c r="B108" s="32"/>
     </row>
     <row r="109" spans="1:2">
-      <c r="A109" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="B109" s="12"/>
+      <c r="A109" s="11"/>
+      <c r="B109" s="32"/>
     </row>
     <row r="110" spans="1:2">
-      <c r="A110" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="B110" s="12"/>
+      <c r="A110" s="11"/>
+      <c r="B110" s="32"/>
     </row>
     <row r="111" spans="1:2">
-      <c r="A111" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="B111" s="12"/>
+      <c r="A111" s="11"/>
+      <c r="B111" s="32"/>
     </row>
     <row r="112" spans="1:2">
-      <c r="A112" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="B112" s="12"/>
+      <c r="A112" s="11"/>
+      <c r="B112" s="32"/>
     </row>
     <row r="113" spans="1:2">
-      <c r="A113" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="B113" s="12"/>
+      <c r="A113" s="11"/>
+      <c r="B113" s="32"/>
     </row>
     <row r="114" spans="1:2">
-      <c r="A114" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="B114" s="12"/>
+      <c r="A114" s="11"/>
+      <c r="B114" s="32"/>
     </row>
     <row r="115" spans="1:2">
-      <c r="A115" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="B115" s="12"/>
+      <c r="A115" s="11"/>
+      <c r="B115" s="32"/>
     </row>
     <row r="116" spans="1:2">
-      <c r="A116" s="23"/>
+      <c r="A116" s="22"/>
     </row>
     <row r="117" spans="1:2">
-      <c r="A117" s="23"/>
+      <c r="A117" s="22"/>
     </row>
     <row r="118" spans="1:2">
-      <c r="A118" s="23"/>
+      <c r="A118" s="22"/>
     </row>
     <row r="119" spans="1:2">
-      <c r="A119" s="23"/>
+      <c r="A119" s="22"/>
     </row>
     <row r="120" spans="1:2">
-      <c r="A120" s="23"/>
+      <c r="A120" s="22"/>
     </row>
     <row r="121" spans="1:2">
-      <c r="A121" s="23"/>
+      <c r="A121" s="22"/>
     </row>
     <row r="122" spans="1:2">
-      <c r="A122" s="23"/>
+      <c r="A122" s="22"/>
     </row>
     <row r="123" spans="1:2">
-      <c r="A123" s="23"/>
+      <c r="A123" s="22"/>
     </row>
     <row r="124" spans="1:2">
-      <c r="A124" s="23"/>
+      <c r="A124" s="22"/>
     </row>
     <row r="125" spans="1:2">
-      <c r="A125" s="23"/>
+      <c r="A125" s="22"/>
     </row>
     <row r="126" spans="1:2">
-      <c r="A126" s="23"/>
+      <c r="A126" s="22"/>
     </row>
     <row r="127" spans="1:2">
-      <c r="A127" s="23"/>
+      <c r="A127" s="22"/>
     </row>
     <row r="128" spans="1:2">
-      <c r="A128" s="23"/>
+      <c r="A128" s="22"/>
     </row>
     <row r="129" spans="1:1">
-      <c r="A129" s="23"/>
+      <c r="A129" s="22"/>
     </row>
     <row r="130" spans="1:1">
-      <c r="A130" s="23"/>
+      <c r="A130" s="22"/>
     </row>
     <row r="131" spans="1:1">
-      <c r="A131" s="23"/>
+      <c r="A131" s="22"/>
     </row>
     <row r="132" spans="1:1">
-      <c r="A132" s="23"/>
+      <c r="A132" s="22"/>
     </row>
     <row r="133" spans="1:1">
-      <c r="A133" s="23"/>
+      <c r="A133" s="22"/>
     </row>
     <row r="134" spans="1:1">
-      <c r="A134" s="23"/>
+      <c r="A134" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>